<commit_message>
add oled main menu
</commit_message>
<xml_diff>
--- a/Docs/12864_OLED界面设置.xlsx
+++ b/Docs/12864_OLED界面设置.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24345" windowHeight="12615"/>
+    <workbookView windowWidth="25200" windowHeight="12015"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="55">
   <si>
     <t>8*8</t>
   </si>
@@ -168,10 +168,19 @@
     <t>隔</t>
   </si>
   <si>
-    <t>℃</t>
-  </si>
-  <si>
-    <t>C</t>
+    <t>=</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>/</t>
   </si>
 </sst>
 </file>
@@ -179,12 +188,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="31">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,7 +243,31 @@
     </font>
     <font>
       <b/>
-      <sz val="22"/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="48"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="48"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -243,6 +276,14 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="72"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -264,31 +305,15 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -299,13 +324,6 @@
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -323,24 +341,48 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -371,14 +413,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -386,21 +428,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -427,192 +461,198 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -706,17 +746,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -762,11 +807,24 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -794,166 +852,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="29" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1062,17 +1111,71 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1422,10 +1525,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AR53"/>
+  <dimension ref="A1:AW63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="AA57" sqref="AA57"/>
+      <selection activeCell="AO59" sqref="AO59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.75" defaultRowHeight="26.25" customHeight="1"/>
@@ -1924,7 +2027,7 @@
       <c r="Q11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="AM11" s="39"/>
+      <c r="AM11" s="46"/>
     </row>
     <row r="12" customHeight="1" spans="1:17">
       <c r="A12" s="3"/>
@@ -2534,314 +2637,375 @@
       <c r="AF26" s="20"/>
       <c r="AG26" s="20"/>
     </row>
+    <row r="40" customHeight="1" spans="25:25">
+      <c r="Y40" s="36"/>
+    </row>
     <row r="45" customHeight="1" spans="29:44">
-      <c r="AC45" s="1" t="s">
+      <c r="AC45" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="AD45" s="1" t="s">
+      <c r="AD45" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="AE45" s="1" t="s">
+      <c r="AE45" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="AF45" s="1" t="s">
+      <c r="AF45" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="AG45" s="1" t="s">
+      <c r="AG45" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="AH45" s="1" t="s">
+      <c r="AH45" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="AI45" s="1" t="s">
+      <c r="AI45" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="AJ45" s="1" t="s">
+      <c r="AJ45" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="AK45" s="1" t="s">
+      <c r="AK45" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="AL45" s="1" t="s">
+      <c r="AL45" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="AM45" s="1" t="s">
+      <c r="AM45" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="AN45" s="1" t="s">
+      <c r="AN45" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="AO45" s="1" t="s">
+      <c r="AO45" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="AP45" s="1" t="s">
+      <c r="AP45" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="AQ45" s="1" t="s">
+      <c r="AQ45" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="AR45" s="1" t="s">
+      <c r="AR45" s="53" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="46" customHeight="1" spans="29:44">
-      <c r="AC46" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD46" s="17" t="s">
+      <c r="AC46" s="39"/>
+      <c r="AD46" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE46" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF46" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="AE46" s="37" t="s">
+      <c r="AG46" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH46" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI46" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ46" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="AK46" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="AL46" s="47"/>
+      <c r="AM46" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="AN46" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO46" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="AP46" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ46" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="AR46" s="40" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" customHeight="1" spans="29:49">
+      <c r="AC47" s="39"/>
+      <c r="AD47" s="40"/>
+      <c r="AE47" s="40"/>
+      <c r="AF47" s="40"/>
+      <c r="AG47" s="40"/>
+      <c r="AH47" s="40"/>
+      <c r="AI47" s="40"/>
+      <c r="AJ47" s="40"/>
+      <c r="AK47" s="40"/>
+      <c r="AL47" s="47"/>
+      <c r="AM47" s="40"/>
+      <c r="AN47" s="40"/>
+      <c r="AO47" s="40"/>
+      <c r="AP47" s="40"/>
+      <c r="AQ47" s="40"/>
+      <c r="AR47" s="40"/>
+      <c r="AW47" s="2"/>
+    </row>
+    <row r="48" customHeight="1" spans="29:44">
+      <c r="AC48" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD48" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE48" s="43"/>
+      <c r="AF48" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG48" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH48" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="AI48" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="AJ48" s="43"/>
+      <c r="AK48" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="AL48" s="48"/>
+      <c r="AM48" s="48"/>
+      <c r="AO48" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="AP48" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="AQ48" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="AR48" s="43"/>
+    </row>
+    <row r="49" customHeight="1" spans="29:44">
+      <c r="AC49" s="41"/>
+      <c r="AD49" s="42"/>
+      <c r="AE49" s="43"/>
+      <c r="AF49" s="41"/>
+      <c r="AG49" s="41"/>
+      <c r="AH49" s="41"/>
+      <c r="AI49" s="41"/>
+      <c r="AJ49" s="43"/>
+      <c r="AK49" s="41"/>
+      <c r="AL49" s="48"/>
+      <c r="AM49" s="48"/>
+      <c r="AO49" s="41"/>
+      <c r="AP49" s="41"/>
+      <c r="AQ49" s="54"/>
+      <c r="AR49" s="43"/>
+    </row>
+    <row r="50" customHeight="1" spans="29:44">
+      <c r="AC50" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD50" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE50" s="57" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF50" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG50" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH50" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="AI50" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ50" s="43"/>
+      <c r="AK50" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL50" s="48"/>
+      <c r="AM50" s="49"/>
+      <c r="AN50" s="50"/>
+      <c r="AO50" s="55"/>
+      <c r="AP50" s="55"/>
+      <c r="AQ50" s="55"/>
+      <c r="AR50" s="55"/>
+    </row>
+    <row r="51" customHeight="1" spans="29:44">
+      <c r="AC51" s="41"/>
+      <c r="AD51" s="42"/>
+      <c r="AE51" s="44"/>
+      <c r="AF51" s="41"/>
+      <c r="AG51" s="41"/>
+      <c r="AH51" s="41"/>
+      <c r="AI51" s="41"/>
+      <c r="AJ51" s="43"/>
+      <c r="AK51" s="41"/>
+      <c r="AL51" s="48"/>
+      <c r="AM51" s="49"/>
+      <c r="AN51" s="50"/>
+      <c r="AO51" s="55"/>
+      <c r="AP51" s="55"/>
+      <c r="AQ51" s="55"/>
+      <c r="AR51" s="55"/>
+    </row>
+    <row r="52" customHeight="1" spans="29:44">
+      <c r="AC52" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD52" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE52" s="41"/>
+      <c r="AF52" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="AF46" s="37" t="s">
+      <c r="AG52" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH52" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI52" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ52" s="43"/>
+      <c r="AK52" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="AL52" s="48"/>
+      <c r="AM52" s="49"/>
+      <c r="AN52" s="50"/>
+      <c r="AO52" s="55"/>
+      <c r="AP52" s="55"/>
+      <c r="AQ52" s="55"/>
+      <c r="AR52" s="55"/>
+    </row>
+    <row r="53" customHeight="1" spans="29:44">
+      <c r="AC53" s="41"/>
+      <c r="AD53" s="42"/>
+      <c r="AE53" s="41"/>
+      <c r="AF53" s="41"/>
+      <c r="AG53" s="41"/>
+      <c r="AH53" s="41"/>
+      <c r="AI53" s="41"/>
+      <c r="AJ53" s="43"/>
+      <c r="AK53" s="41"/>
+      <c r="AL53" s="48"/>
+      <c r="AM53" s="49"/>
+      <c r="AN53" s="50"/>
+      <c r="AO53" s="55"/>
+      <c r="AP53" s="55"/>
+      <c r="AQ53" s="55"/>
+      <c r="AR53" s="55"/>
+    </row>
+    <row r="55" customHeight="1" spans="1:1">
+      <c r="A55" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" customHeight="1" spans="29:36">
+      <c r="AC56" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="AG46" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="AH46" s="37" t="s">
+      <c r="AD56" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE56" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF56" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="AI46" s="37" t="s">
+      <c r="AG56" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH56" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI56" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="AJ46" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="AK46" s="37" t="s">
-        <v>44</v>
-      </c>
-      <c r="AL46" s="37"/>
-      <c r="AM46" s="37" t="s">
+      <c r="AJ56" s="45" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" customHeight="1" spans="29:36">
+      <c r="AC57" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="AN46" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="AO46" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="AP46" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="AQ46" s="37" t="s">
-        <v>50</v>
-      </c>
-      <c r="AR46" s="37"/>
-    </row>
-    <row r="47" customHeight="1" spans="29:44">
-      <c r="AC47" s="38"/>
-      <c r="AD47" s="18"/>
-      <c r="AE47" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="AF47" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG47" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="AH47" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI47" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJ47" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="AK47" s="37"/>
-      <c r="AL47" s="37"/>
-      <c r="AM47" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="AN47" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="AO47" s="37" t="s">
+      <c r="AD57" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE57" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="AP47" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="AQ47" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="AR47" s="37"/>
-    </row>
-    <row r="48" customHeight="1" spans="29:44">
-      <c r="AC48" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD48" s="7"/>
-      <c r="AE48" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="AF48" s="7"/>
-      <c r="AG48" s="17" t="s">
+      <c r="AF57" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG57" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH57" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="AH48" s="17"/>
-      <c r="AI48" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ48" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK48" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="AL48" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="AM48" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="AN48" s="17"/>
-      <c r="AO48" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="AP48" s="17"/>
-      <c r="AQ48" s="37"/>
-      <c r="AR48" s="37"/>
-    </row>
-    <row r="49" customHeight="1" spans="29:44">
-      <c r="AC49" s="9"/>
-      <c r="AD49" s="10"/>
-      <c r="AE49" s="9"/>
-      <c r="AF49" s="10"/>
-      <c r="AG49" s="18"/>
-      <c r="AH49" s="18"/>
-      <c r="AI49" s="18"/>
-      <c r="AJ49" s="18"/>
-      <c r="AK49" s="18"/>
-      <c r="AL49" s="18"/>
-      <c r="AM49" s="18"/>
-      <c r="AN49" s="18"/>
-      <c r="AO49" s="20"/>
-      <c r="AP49" s="18"/>
-      <c r="AQ49" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="AR49" s="37" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" customHeight="1" spans="29:44">
-      <c r="AC50" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD50" s="7"/>
-      <c r="AE50" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF50" s="7"/>
-      <c r="AG50" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="AH50" s="17"/>
-      <c r="AI50" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ50" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK50" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="AL50" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="AM50" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="AN50" s="17"/>
-      <c r="AO50" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="AP50" s="17"/>
-      <c r="AQ50" s="37"/>
-      <c r="AR50" s="37"/>
-    </row>
-    <row r="51" customHeight="1" spans="29:44">
-      <c r="AC51" s="9"/>
-      <c r="AD51" s="10"/>
-      <c r="AE51" s="9"/>
-      <c r="AF51" s="10"/>
-      <c r="AG51" s="18"/>
-      <c r="AH51" s="18"/>
-      <c r="AI51" s="18"/>
-      <c r="AJ51" s="18"/>
-      <c r="AK51" s="18"/>
-      <c r="AL51" s="18"/>
-      <c r="AM51" s="18"/>
-      <c r="AN51" s="18"/>
-      <c r="AO51" s="18"/>
-      <c r="AP51" s="18"/>
-      <c r="AQ51" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="AR51" s="37" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="52" customHeight="1" spans="29:44">
-      <c r="AC52" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="AD52" s="7"/>
-      <c r="AE52" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="AF52" s="7"/>
-      <c r="AG52" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="AH52" s="17"/>
-      <c r="AI52" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ52" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK52" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="AL52" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="AM52" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="AN52" s="17"/>
-      <c r="AO52" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="AP52" s="17"/>
-      <c r="AQ52" s="37"/>
-      <c r="AR52" s="37"/>
-    </row>
-    <row r="53" customHeight="1" spans="29:44">
-      <c r="AC53" s="9"/>
-      <c r="AD53" s="10"/>
-      <c r="AE53" s="9"/>
-      <c r="AF53" s="10"/>
-      <c r="AG53" s="18"/>
-      <c r="AH53" s="18"/>
-      <c r="AI53" s="18"/>
-      <c r="AJ53" s="18"/>
-      <c r="AK53" s="18"/>
-      <c r="AL53" s="18"/>
-      <c r="AM53" s="18"/>
-      <c r="AN53" s="18"/>
-      <c r="AO53" s="18"/>
-      <c r="AP53" s="18"/>
-      <c r="AQ53" s="37"/>
-      <c r="AR53" s="37"/>
+      <c r="AI57" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="AJ57" s="45" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" customHeight="1" spans="37:44">
+      <c r="AK60" s="51"/>
+      <c r="AL60" s="44"/>
+      <c r="AM60" s="41"/>
+      <c r="AN60" s="41"/>
+      <c r="AO60" s="41"/>
+      <c r="AP60" s="41"/>
+      <c r="AR60" s="41"/>
+    </row>
+    <row r="61" customHeight="1" spans="37:44">
+      <c r="AK61" s="52"/>
+      <c r="AL61" s="44"/>
+      <c r="AM61" s="41"/>
+      <c r="AN61" s="41"/>
+      <c r="AO61" s="41"/>
+      <c r="AP61" s="41"/>
+      <c r="AR61" s="41"/>
+    </row>
+    <row r="62" customHeight="1" spans="37:44">
+      <c r="AK62" s="51"/>
+      <c r="AL62" s="41"/>
+      <c r="AM62" s="41"/>
+      <c r="AN62" s="41"/>
+      <c r="AO62" s="41"/>
+      <c r="AP62" s="41"/>
+      <c r="AR62" s="41"/>
+    </row>
+    <row r="63" customHeight="1" spans="37:44">
+      <c r="AK63" s="52"/>
+      <c r="AL63" s="41"/>
+      <c r="AM63" s="41"/>
+      <c r="AN63" s="41"/>
+      <c r="AO63" s="41"/>
+      <c r="AP63" s="41"/>
+      <c r="AR63" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="167">
+  <mergeCells count="183">
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="B23:B24"/>
@@ -2924,17 +3088,25 @@
     <mergeCell ref="AC21:AC22"/>
     <mergeCell ref="AC23:AC24"/>
     <mergeCell ref="AC25:AC26"/>
-    <mergeCell ref="AC46:AC47"/>
+    <mergeCell ref="AC48:AC49"/>
+    <mergeCell ref="AC50:AC51"/>
+    <mergeCell ref="AC52:AC53"/>
     <mergeCell ref="AD1:AD2"/>
     <mergeCell ref="AD3:AD4"/>
     <mergeCell ref="AD5:AD6"/>
     <mergeCell ref="AD7:AD8"/>
     <mergeCell ref="AD19:AD20"/>
     <mergeCell ref="AD46:AD47"/>
+    <mergeCell ref="AD48:AD49"/>
+    <mergeCell ref="AD50:AD51"/>
+    <mergeCell ref="AD52:AD53"/>
     <mergeCell ref="AE1:AE2"/>
     <mergeCell ref="AE3:AE4"/>
     <mergeCell ref="AE7:AE8"/>
     <mergeCell ref="AE25:AE26"/>
+    <mergeCell ref="AE46:AE47"/>
+    <mergeCell ref="AE50:AE51"/>
+    <mergeCell ref="AE52:AE53"/>
     <mergeCell ref="AF1:AF2"/>
     <mergeCell ref="AF3:AF4"/>
     <mergeCell ref="AF7:AF8"/>
@@ -2942,39 +3114,53 @@
     <mergeCell ref="AF21:AF22"/>
     <mergeCell ref="AF23:AF24"/>
     <mergeCell ref="AF25:AF26"/>
+    <mergeCell ref="AF46:AF47"/>
+    <mergeCell ref="AF48:AF49"/>
+    <mergeCell ref="AF50:AF51"/>
+    <mergeCell ref="AF52:AF53"/>
     <mergeCell ref="AG21:AG22"/>
     <mergeCell ref="AG23:AG24"/>
     <mergeCell ref="AG25:AG26"/>
+    <mergeCell ref="AG46:AG47"/>
     <mergeCell ref="AG48:AG49"/>
     <mergeCell ref="AG50:AG51"/>
     <mergeCell ref="AG52:AG53"/>
+    <mergeCell ref="AH46:AH47"/>
     <mergeCell ref="AH48:AH49"/>
     <mergeCell ref="AH50:AH51"/>
     <mergeCell ref="AH52:AH53"/>
+    <mergeCell ref="AI46:AI47"/>
     <mergeCell ref="AI48:AI49"/>
     <mergeCell ref="AI50:AI51"/>
     <mergeCell ref="AI52:AI53"/>
-    <mergeCell ref="AJ48:AJ49"/>
-    <mergeCell ref="AJ50:AJ51"/>
-    <mergeCell ref="AJ52:AJ53"/>
+    <mergeCell ref="AJ46:AJ47"/>
+    <mergeCell ref="AK46:AK47"/>
     <mergeCell ref="AK48:AK49"/>
     <mergeCell ref="AK50:AK51"/>
     <mergeCell ref="AK52:AK53"/>
-    <mergeCell ref="AL48:AL49"/>
-    <mergeCell ref="AL50:AL51"/>
-    <mergeCell ref="AL52:AL53"/>
-    <mergeCell ref="AM48:AM49"/>
-    <mergeCell ref="AM50:AM51"/>
-    <mergeCell ref="AM52:AM53"/>
-    <mergeCell ref="AN48:AN49"/>
-    <mergeCell ref="AN50:AN51"/>
-    <mergeCell ref="AN52:AN53"/>
+    <mergeCell ref="AK60:AK61"/>
+    <mergeCell ref="AK62:AK63"/>
+    <mergeCell ref="AL60:AL61"/>
+    <mergeCell ref="AL62:AL63"/>
+    <mergeCell ref="AM46:AM47"/>
+    <mergeCell ref="AM60:AM61"/>
+    <mergeCell ref="AM62:AM63"/>
+    <mergeCell ref="AN46:AN47"/>
+    <mergeCell ref="AN60:AN61"/>
+    <mergeCell ref="AN62:AN63"/>
+    <mergeCell ref="AO46:AO47"/>
     <mergeCell ref="AO48:AO49"/>
-    <mergeCell ref="AO50:AO51"/>
-    <mergeCell ref="AO52:AO53"/>
+    <mergeCell ref="AO60:AO61"/>
+    <mergeCell ref="AO62:AO63"/>
+    <mergeCell ref="AP46:AP47"/>
     <mergeCell ref="AP48:AP49"/>
-    <mergeCell ref="AP50:AP51"/>
-    <mergeCell ref="AP52:AP53"/>
+    <mergeCell ref="AP60:AP61"/>
+    <mergeCell ref="AP62:AP63"/>
+    <mergeCell ref="AQ46:AQ47"/>
+    <mergeCell ref="AQ48:AQ49"/>
+    <mergeCell ref="AR46:AR47"/>
+    <mergeCell ref="AR60:AR61"/>
+    <mergeCell ref="AR62:AR63"/>
     <mergeCell ref="E3:F4"/>
     <mergeCell ref="G3:H4"/>
     <mergeCell ref="I3:J4"/>
@@ -3003,12 +3189,6 @@
     <mergeCell ref="U23:V24"/>
     <mergeCell ref="S25:T26"/>
     <mergeCell ref="U25:V26"/>
-    <mergeCell ref="AC48:AD49"/>
-    <mergeCell ref="AE48:AF49"/>
-    <mergeCell ref="AC50:AD51"/>
-    <mergeCell ref="AE50:AF51"/>
-    <mergeCell ref="AC52:AD53"/>
-    <mergeCell ref="AE52:AF53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>

</xml_diff>